<commit_message>
Creación de transaccion pago de tc propia mayor a la deuda
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/pagos/TarjetaCreditoPropia.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/pagos/TarjetaCreditoPropia.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19320"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>406-738430-25</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>invictus10</t>
+  </si>
+  <si>
+    <t>*7806</t>
   </si>
 </sst>
 </file>
@@ -611,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -892,14 +901,76 @@
         <v>52</v>
       </c>
     </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="10"/>
+      <c r="U5" s="14"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1"/>
     <hyperlink ref="N3" r:id="rId2"/>
     <hyperlink ref="N4" r:id="rId3"/>
+    <hyperlink ref="N5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>